<commit_message>
Add the previous data analysis figures.
</commit_message>
<xml_diff>
--- a/data40.xlsx
+++ b/data40.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dongshengyang/Downloads/iMacResearch/github/CameraControl/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/y.dongdong/Downloads/DongHub/Github/CameraControl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562B53A8-C3FB-C441-AE51-D57482BBE4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB88A4B0-1B12-5044-AC8A-86C7311E9B37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17780" yWindow="460" windowWidth="11020" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -1699,12 +1699,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1757,7 +1764,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1773,7 +1780,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2071,29 +2078,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:NM45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BA1" zoomScale="164" zoomScaleNormal="81" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BP12" sqref="BP12"/>
+    <sheetView tabSelected="1" topLeftCell="CQ1" zoomScale="115" zoomScaleNormal="81" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="CR50" sqref="CR50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="20" max="20" width="11.83203125" customWidth="1"/>
-    <col min="21" max="21" width="11.1640625" customWidth="1"/>
-    <col min="22" max="22" width="11.33203125" customWidth="1"/>
-    <col min="23" max="23" width="11.1640625" customWidth="1"/>
-    <col min="24" max="33" width="8.83203125" customWidth="1"/>
-    <col min="34" max="34" width="6.1640625" customWidth="1"/>
-    <col min="35" max="35" width="5.1640625" customWidth="1"/>
-    <col min="36" max="36" width="8.83203125" customWidth="1"/>
-    <col min="37" max="37" width="18.33203125" customWidth="1"/>
-    <col min="38" max="40" width="8.83203125" customWidth="1"/>
-    <col min="42" max="47" width="8.83203125" customWidth="1"/>
-    <col min="48" max="48" width="13.33203125" customWidth="1"/>
-    <col min="49" max="377" width="8.83203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.1640625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:377" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:377">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3226,7 +3218,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="2" spans="1:377" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:377">
       <c r="A2" s="3" t="s">
         <v>377</v>
       </c>
@@ -4359,7 +4351,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="3" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:377" ht="48">
       <c r="A3" s="1">
         <v>44586.710844907408</v>
       </c>
@@ -5492,7 +5484,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="4" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:377" ht="48">
       <c r="A4" s="1">
         <v>44586.710335648146</v>
       </c>
@@ -6625,7 +6617,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="5" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:377" ht="48">
       <c r="A5" s="1">
         <v>44586.710729166669</v>
       </c>
@@ -7758,7 +7750,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="6" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:377" ht="48">
       <c r="A6" s="1">
         <v>44586.710555555554</v>
       </c>
@@ -8891,7 +8883,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="7" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:377" ht="48">
       <c r="A7" s="1">
         <v>44586.712280092594</v>
       </c>
@@ -10024,7 +10016,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="8" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:377" ht="48">
       <c r="A8" s="1">
         <v>44586.711701388886</v>
       </c>
@@ -11157,7 +11149,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="9" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:377" ht="32">
       <c r="A9" s="1">
         <v>44586.71434027778</v>
       </c>
@@ -12290,7 +12282,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="10" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:377" ht="48">
       <c r="A10" s="1">
         <v>44586.7112037037</v>
       </c>
@@ -13423,7 +13415,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="11" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:377" ht="48">
       <c r="A11" s="1">
         <v>44586.709976851853</v>
       </c>
@@ -14556,7 +14548,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="12" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:377" ht="48">
       <c r="A12" s="1">
         <v>44586.709756944445</v>
       </c>
@@ -15689,7 +15681,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="13" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:377" ht="32">
       <c r="A13" s="1">
         <v>44586.710347222222</v>
       </c>
@@ -16822,7 +16814,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="14" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:377" ht="48">
       <c r="A14" s="1">
         <v>44586.711944444447</v>
       </c>
@@ -17955,7 +17947,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="15" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:377" ht="48">
       <c r="A15" s="1">
         <v>44586.710497685184</v>
       </c>
@@ -19088,7 +19080,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="16" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:377" ht="48">
       <c r="A16" s="1">
         <v>44586.711631944447</v>
       </c>
@@ -20221,7 +20213,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="17" spans="1:377" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:377" ht="32">
       <c r="A17" s="1">
         <v>44586.716469907406</v>
       </c>
@@ -21354,7 +21346,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="18" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:377" ht="48">
       <c r="A18" s="1">
         <v>44586.715590277781</v>
       </c>
@@ -22487,7 +22479,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="19" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:377" ht="48">
       <c r="A19" s="1">
         <v>44586.709675925929</v>
       </c>
@@ -23620,7 +23612,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="20" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:377" ht="48">
       <c r="A20" s="1">
         <v>44586.725891203707</v>
       </c>
@@ -24753,7 +24745,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="21" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:377" ht="48">
       <c r="A21" s="1">
         <v>44586.727951388886</v>
       </c>
@@ -25886,7 +25878,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="22" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:377" ht="48">
       <c r="A22" s="1">
         <v>44586.710821759261</v>
       </c>
@@ -27019,7 +27011,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="23" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:377" ht="48">
       <c r="A23" s="1">
         <v>44586.735763888886</v>
       </c>
@@ -28152,7 +28144,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="24" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:377" ht="32">
       <c r="A24" s="1">
         <v>44586.721944444442</v>
       </c>
@@ -29285,7 +29277,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="25" spans="1:377" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:377" ht="32">
       <c r="A25" s="1">
         <v>44586.728136574071</v>
       </c>
@@ -30418,7 +30410,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="26" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:377" ht="48">
       <c r="A26" s="1">
         <v>44586.734131944446</v>
       </c>
@@ -31551,7 +31543,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="27" spans="1:377" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:377" ht="48">
       <c r="A27" s="1">
         <v>44586.752766203703</v>
       </c>
@@ -32684,7 +32676,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="28" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:377" ht="48">
       <c r="A28" s="1">
         <v>44586.751168981478</v>
       </c>
@@ -33817,7 +33809,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="29" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:377" ht="48">
       <c r="A29" s="1">
         <v>44586.752268518518</v>
       </c>
@@ -34950,7 +34942,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="30" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:377" ht="48">
       <c r="A30" s="1">
         <v>44586.752581018518</v>
       </c>
@@ -36083,7 +36075,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="31" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:377" ht="48">
       <c r="A31" s="1">
         <v>44586.752060185187</v>
       </c>
@@ -37216,7 +37208,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="32" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:377" ht="48">
       <c r="A32" s="1">
         <v>44586.755844907406</v>
       </c>
@@ -38349,7 +38341,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="33" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:377" ht="48">
       <c r="A33" s="1">
         <v>44586.753541666665</v>
       </c>
@@ -39482,7 +39474,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="34" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:377" ht="48">
       <c r="A34" s="1">
         <v>44586.755127314813</v>
       </c>
@@ -40615,7 +40607,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="35" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:377" ht="32">
       <c r="A35" s="1">
         <v>44586.755023148151</v>
       </c>
@@ -41748,7 +41740,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="36" spans="1:377" ht="32" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:377" ht="32">
       <c r="A36" s="1">
         <v>44586.757268518515</v>
       </c>
@@ -42881,7 +42873,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="37" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:377" ht="48">
       <c r="A37" s="1">
         <v>44586.753599537034</v>
       </c>
@@ -44014,7 +44006,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="38" spans="1:377" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:377" ht="31" customHeight="1">
       <c r="A38" s="1">
         <v>44586.771203703705</v>
       </c>
@@ -45147,7 +45139,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="39" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:377" ht="48">
       <c r="A39" s="1">
         <v>44586.753368055557</v>
       </c>
@@ -46280,7 +46272,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="40" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:377" ht="48">
       <c r="A40" s="1">
         <v>44587.514699074076</v>
       </c>
@@ -47413,7 +47405,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="41" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:377" ht="48">
       <c r="A41" s="1">
         <v>44587.530590277776</v>
       </c>
@@ -48546,7 +48538,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="42" spans="1:377" ht="48" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:377" ht="48">
       <c r="A42" s="1">
         <v>44588.459467592591</v>
       </c>
@@ -49679,7 +49671,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="44" spans="1:377" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:377" s="6" customFormat="1" ht="16">
       <c r="S44" s="7" t="s">
         <v>543</v>
       </c>
@@ -51112,7 +51104,7 @@
         <v>5.0250000000000004</v>
       </c>
     </row>
-    <row r="45" spans="1:377" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:377" s="6" customFormat="1" ht="32">
       <c r="S45" s="7" t="s">
         <v>544</v>
       </c>
@@ -52547,6 +52539,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:NM42" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="C1:C42 D1:D42 G1:G42 I1:I42 J1:J42 K1:K42 L1:L42 M1:M42 P1:P42 Q1:Q42 R1:R42 S1:S42 T1 U1 V1 W1 X1 Y1:Y2 Z1:Z2 AA1:AA2 AB1 AC1:AC2 AD1:AD2 AE1 AF1:AF2 AG1:AG2 AH1 AI1 AJ1 AK1 AL1 AM1 AN1 AO1 AP1 AQ1 AR1 AS1 AT1 AU1 AV1 AW1 AX1 AY1 AZ1 BA1 BB1 BC1 BD1 BE1 BF1 BG1 BH1 BI1 BJ1 BK1 BL1 BM1 BN1 BO1 BP1 BQ1 BR1 BS1 BT1 BU1 BV1 BW1 BX1 BY1 BZ1 CA1 CB1 CC1 CD1 CE1 CF1 CG1 CH1 CI1 CJ1 CK1 CL1 CM1 CN1 CO1 CP1 CQ1 CR1 CS1 CT1 CU1 CV1 CW1 CX1 CY1 CZ1 DA1 DB1 DC1 DD1 DE1 DF1 DG1 DH1 DI1 DJ1 DK1 DL1 DM1 DN1 DO1 DP1 DQ1 DR1 DS1 DT1 DU1 DV1 DW1 DX1 DY1 DZ1 EA1 EB1 EC1 ED1 EE1 EF1 EG1 EH1 EI1 EJ1 EK1 EL1 EM1 EN1 EO1 EP1 EQ1 ER1 ES1 ET1 EU1 EV1 EW1 EX1 EY1 EZ1 FA1 FB1 FC1 FD1 FE1 FF1 FG1 FH1 FI1 FJ1 FK1 FL1 FM1 FN1 FO1 FP1 FQ1 FR1 FS1 FT1 FU1 FV1 FW1 FX1 FY1 FZ1 GA1 GB1 GC1 GD1 GE1 GF1 GG1 GH1 GI1 GJ1 GK1 GL1 GM1 GN1 GO1 GP1 GQ1 GR1 GS1 GT1 GU1 GV1 GW1 GX1 GY1 GZ1 HA1 HB1 HC1 HD1 HE1 HF1 HG1 HH1 HI1 HJ1 HK1 HL1 HM1 HN1 HO1 HP1 HQ1 HR1 HS1 HT1 HU1 HV1 HW1 HX1 HY1 HZ1 IA1 IB1 IC1 ID1 IE1 IF1 IG1 IH1 II1 IJ1 IK1 IL1 IM1 IN1 IO1 IP1 IQ1 IR1 IS1 IT1 IU1 IV1 IW1 IX1 IY1 IZ1 JA1 JB1 JC1 JD1 JE1 JF1 JG1 JH1 JI1 JJ1 JK1 JL1 JM1 JN1 JO1 JP1 JQ1 JR1 JS1 JT1 JU1 JV1 JW1 JX1 JY1 JZ1 KA1 KB1 KC1 KD1 KE1 KF1 KG1 KH1 KI1 KJ1 KK1 KL1 KM1 KN1 KO1 KP1 KQ1 KR1 KS1 KT1 KU1 KV1 KW1 KX1 KY1 KZ1 LA1 LB1 LC1 LD1 LE1 LF1 LG1 LH1 LI1 LJ1 LK1 LL1 LM1 LN1 LO1 LP1 LQ1 LR1 LS1 LT1 LU1 LV1 LW1 LX1 LY1 LZ1 MA1 MB1 MC1 MD1 ME1 MF1 MG1 MH1 MI1 MJ1 MK1 ML1 MM1 MN1 MO1 MP1 MQ1 MR1 MS1 MT1 MU1 MV1 MW1 MX1 MY1 MZ1 NA1 NB1 NC1 ND1 NE1 NF1 NG1 NH1 NI1 NJ1 NK1 NL1 NM1:NM42" numberStoredAsText="1"/>

</xml_diff>